<commit_message>
export all marketmodelevolver functions to Excel (894/1114)
</commit_message>
<xml_diff>
--- a/UnitTests/Tests/MarketModelEvolvers.xlsx
+++ b/UnitTests/Tests/MarketModelEvolvers.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\reposit\QuantLibXL\UnitTests\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21900F73-E35E-40F2-B04C-470419F9E8EE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="75" yWindow="120" windowWidth="19485" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,14 +18,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="UNIT_TEST" localSheetId="0">Sheet1!$A$3:$G$3</definedName>
+    <definedName name="UNIT_TEST" localSheetId="0">Sheet1!$A$3:$E$9</definedName>
   </definedNames>
   <calcPr calcId="171027" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Function</t>
   </si>
@@ -50,22 +51,25 @@
     <t>Actual</t>
   </si>
   <si>
-    <t>correlations</t>
-  </si>
-  <si>
-    <t>evolution</t>
-  </si>
-  <si>
-    <t>piecewiseconstantvariance</t>
-  </si>
-  <si>
-    <t>curvestate</t>
-  </si>
-  <si>
-    <t>flat vol</t>
-  </si>
-  <si>
     <t>qlForwardRatePc</t>
+  </si>
+  <si>
+    <t>qlForwardRateIpc</t>
+  </si>
+  <si>
+    <t>qlForwardRateNormalPc</t>
+  </si>
+  <si>
+    <t>qlMarketModelEvolverStartNewPath</t>
+  </si>
+  <si>
+    <t>qlMarketModelEvolverAdvanceStep</t>
+  </si>
+  <si>
+    <t>qlMarketModelEvolverCurrentStep</t>
+  </si>
+  <si>
+    <t>qlMarketModelEvolverNumeraires</t>
   </si>
 </sst>
 </file>
@@ -457,7 +461,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -469,11 +473,9 @@
     <col min="1" max="1" width="46" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -489,9 +491,8 @@
       <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -507,301 +508,117 @@
       <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>8</v>
+      </c>
+      <c r="B3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="D3" s="3" t="str">
         <f>IF(ISERROR(B3),"ERROR",IF(ISERROR(C3),"FAIL",IF(B3=C3,"PASS","FAIL")))</f>
-        <v>PASS</v>
+        <v>ERROR</v>
       </c>
       <c r="E3" t="e">
-        <f>_xll.qlForwardRatePc("mme01")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="str">
-        <f>_xll.qlTimeHomogeneousForwardCorrelation(,I3:L6,H10:L10)</f>
-        <v>obj_00000#0031</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-      <c r="K3">
-        <v>3</v>
-      </c>
-      <c r="L3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F4" t="s">
+        <f>_xll.qlForwardRatePc()</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="G4" t="str">
-        <f>_xll.qlEvolutionDescription(,H10:L10,H10:K10)</f>
-        <v>obj_00001#0055</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="I4">
-        <v>4</v>
-      </c>
-      <c r="J4">
-        <v>5</v>
-      </c>
-      <c r="K4">
-        <v>6</v>
-      </c>
-      <c r="L4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F5" t="s">
+      <c r="B4" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="D4" s="3" t="str">
+        <f t="shared" ref="D4:D9" si="0">IF(ISERROR(B4),"ERROR",IF(ISERROR(C4),"FAIL",IF(B4=C4,"PASS","FAIL")))</f>
+        <v>ERROR</v>
+      </c>
+      <c r="E4" t="e">
+        <f>_xll.qlForwardRateIpc()</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="D5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>ERROR</v>
+      </c>
+      <c r="E5" t="e">
+        <f>_xll.qlForwardRateNormalPc()</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>ERROR</v>
+      </c>
+      <c r="E6" t="e">
+        <f>_xll.qlMarketModelEvolverStartNewPath()</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="G5" t="e">
-        <f>_xll.qlFlatVol("mme03",H11:M11,G3,G4,6,H12:M12,H13:M13)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="I5">
-        <v>7</v>
-      </c>
-      <c r="J5">
-        <v>8</v>
-      </c>
-      <c r="K5">
-        <v>9</v>
-      </c>
-      <c r="L5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" t="str">
-        <f>_xll.qlPiecewiseConstantAbcdVariance(,1,2,3,4,1,"1,2,3")</f>
-        <v>obj_00002#0012</v>
-      </c>
-      <c r="H6">
-        <v>4</v>
-      </c>
-      <c r="I6">
-        <v>10</v>
-      </c>
-      <c r="J6">
-        <v>11</v>
-      </c>
-      <c r="K6">
-        <v>12</v>
-      </c>
-      <c r="L6">
+      <c r="B7" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>ERROR</v>
+      </c>
+      <c r="E7" t="e">
+        <f>_xll.qlMarketModelEvolverAdvanceStep()</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" t="str">
-        <f>_xll.qlCMSwapCurveState(,H10:L10,5)</f>
-        <v>obj_00003#0021</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G8" t="e">
-        <f>_xll.qlCTSMMCapletOriginalCalibration(,G4,G3,G6,,G7)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H10">
-        <v>0.5</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>1.5</v>
-      </c>
-      <c r="K10">
-        <v>2</v>
-      </c>
-      <c r="L10">
-        <v>2.5</v>
-      </c>
-      <c r="M10">
-        <v>3</v>
-      </c>
-      <c r="N10">
-        <v>3.5</v>
-      </c>
-      <c r="O10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H11">
-        <v>0.2</v>
-      </c>
-      <c r="I11">
-        <v>0.2</v>
-      </c>
-      <c r="J11">
-        <v>0.2</v>
-      </c>
-      <c r="K11">
-        <v>0.2</v>
-      </c>
-      <c r="L11">
-        <v>0.2</v>
-      </c>
-      <c r="M11">
-        <v>0.2</v>
-      </c>
-      <c r="N11">
-        <v>0.2</v>
-      </c>
-      <c r="O11">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H12">
-        <v>0.02</v>
-      </c>
-      <c r="I12">
-        <v>0.02</v>
-      </c>
-      <c r="J12">
-        <v>0.02</v>
-      </c>
-      <c r="K12">
-        <v>0.02</v>
-      </c>
-      <c r="L12">
-        <v>0.02</v>
-      </c>
-      <c r="M12">
-        <v>0.02</v>
-      </c>
-      <c r="N12">
-        <v>0.02</v>
-      </c>
-      <c r="O12">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <v>1</v>
-      </c>
-      <c r="M15">
-        <v>1</v>
-      </c>
-      <c r="N15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H16">
-        <v>0.02</v>
-      </c>
-      <c r="I16">
-        <v>0.02</v>
-      </c>
-      <c r="J16">
-        <v>0.02</v>
-      </c>
-      <c r="K16">
-        <v>0.02</v>
-      </c>
-      <c r="L16">
-        <v>0.02</v>
-      </c>
-      <c r="M16">
-        <v>0.02</v>
-      </c>
-      <c r="N16">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="17" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17">
-        <v>0</v>
+      <c r="B8" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="D8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>ERROR</v>
+      </c>
+      <c r="E8" t="e">
+        <f>_xll.qlMarketModelEvolverCurrentStep()</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>ERROR</v>
+      </c>
+      <c r="E9" t="e">
+        <f>_xll.qlMarketModelEvolverNumeraires()</f>
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>